<commit_message>
add product in xls and pdf
</commit_message>
<xml_diff>
--- a/docs/Produits.xlsx
+++ b/docs/Produits.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
-  <workbookPr checkCompatibility="1"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alexandre/Desktop/M2 SID PROJECT/Agents-Fournisseur/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alexandre/Desktop/M2 SID PROJECT/Agents-Fournisseur/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="15360" windowHeight="10480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,20 +29,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
   <si>
     <t>Nom produit</t>
   </si>
   <si>
+    <t>Marque</t>
+  </si>
+  <si>
     <t>Decription produit</t>
   </si>
   <si>
+    <t>Prix produit au kilo/litre</t>
+  </si>
+  <si>
     <t>Catégorie</t>
   </si>
   <si>
     <t>Carotte</t>
   </si>
   <si>
+    <t>Bonduel</t>
+  </si>
+  <si>
     <t>Légume orange riche en protéines</t>
   </si>
   <si>
@@ -52,25 +61,37 @@
     <t>Poireau</t>
   </si>
   <si>
+    <t>Géant Vert</t>
+  </si>
+  <si>
     <t>Légume vert plein de fibre</t>
   </si>
   <si>
     <t>Citrouille</t>
   </si>
   <si>
+    <t>Cascina Belvedere</t>
+  </si>
+  <si>
     <t>Légume orange parfait pour les fêtes d'Halloween</t>
   </si>
   <si>
     <t>Brie</t>
   </si>
   <si>
+    <t>Président</t>
+  </si>
+  <si>
     <t>Fromage de caractère au lait de vache</t>
   </si>
   <si>
     <t>Produit laitier</t>
   </si>
   <si>
-    <t>Conté</t>
+    <t>Comté</t>
+  </si>
+  <si>
+    <t>Entremont</t>
   </si>
   <si>
     <t>Fromage au lait cru</t>
@@ -79,12 +100,18 @@
     <t>Lait</t>
   </si>
   <si>
+    <t>Candia</t>
+  </si>
+  <si>
     <t>Produit laitier semi-écrémé</t>
   </si>
   <si>
     <t>Bière</t>
   </si>
   <si>
+    <t>Chouffe</t>
+  </si>
+  <si>
     <t>Boisson alcoolisée à base d'orge et d'houblon</t>
   </si>
   <si>
@@ -94,18 +121,27 @@
     <t>Eau</t>
   </si>
   <si>
+    <t>Evian</t>
+  </si>
+  <si>
     <t>Eau de source</t>
   </si>
   <si>
     <t>Coca</t>
   </si>
   <si>
+    <t>Coca cola</t>
+  </si>
+  <si>
     <t>Boisson gazeuse sucrée</t>
   </si>
   <si>
     <t>Javel</t>
   </si>
   <si>
+    <t>Monsieur Propre</t>
+  </si>
+  <si>
     <t>Solution liquide oxydante désinfectante et décolorante</t>
   </si>
   <si>
@@ -115,10 +151,16 @@
     <t>Lave vitre</t>
   </si>
   <si>
+    <t>Kärcher</t>
+  </si>
+  <si>
     <t>Solution nettoyante spéciale fenêtre</t>
   </si>
   <si>
-    <t>Paic Citron</t>
+    <t>Liquide vaisselle</t>
+  </si>
+  <si>
+    <t>Paic</t>
   </si>
   <si>
     <t>Liquide vaisselle super dégraissant</t>
@@ -127,6 +169,9 @@
     <t>Parfum</t>
   </si>
   <si>
+    <t>Channel</t>
+  </si>
+  <si>
     <t>Fragrance délicate et boisée</t>
   </si>
   <si>
@@ -136,23 +181,114 @@
     <t>Rouge à lèvre</t>
   </si>
   <si>
+    <t>Velvet</t>
+  </si>
+  <si>
     <t>Produit de cosmétique permettant de souligner les lèvres</t>
   </si>
   <si>
     <t>Fond de teint</t>
   </si>
   <si>
+    <t>Maybelline</t>
+  </si>
+  <si>
     <t>Produit cosmétique permettant d'unifier et de protéger l'épiderme</t>
+  </si>
+  <si>
+    <t>Television HD</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Poste de télévision permettant l'emission et la reception de séquences audiovisuelles</t>
+  </si>
+  <si>
+    <t>High-tech</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>GSM nouvelle génération</t>
+  </si>
+  <si>
+    <t>Rasoir éléctrique</t>
+  </si>
+  <si>
+    <t>Phillips</t>
+  </si>
+  <si>
+    <t>Rasoir performant et plus ergonomique pour un meilleur rasage de la moustache</t>
+  </si>
+  <si>
+    <t>Grand Frais</t>
+  </si>
+  <si>
+    <t>Cassegrin</t>
+  </si>
+  <si>
+    <t>Nos régions ont du talent</t>
+  </si>
+  <si>
+    <t>Coeur de lion</t>
+  </si>
+  <si>
+    <t>Juraflore</t>
+  </si>
+  <si>
+    <t>Lactel</t>
+  </si>
+  <si>
+    <t>Kronenbourg</t>
+  </si>
+  <si>
+    <t>Vittel</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Saint Marc</t>
+  </si>
+  <si>
+    <t>Ecovacs</t>
+  </si>
+  <si>
+    <t>Mir</t>
+  </si>
+  <si>
+    <t>Dior</t>
+  </si>
+  <si>
+    <t>L'Oreal</t>
+  </si>
+  <si>
+    <t>Bourjois</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Wilkinson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,11 +316,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -217,9 +348,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -538,20 +672,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="50.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="65.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,176 +695,627 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>15.05</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7.92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.71</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2">
+        <v>9.23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2">
+        <v>56.48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2">
+        <v>28.9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2">
+        <v>299.99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2">
+        <v>149.9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2">
+        <v>72.040000000000006</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="D20" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D21" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="D22" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D23" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="E23" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+      <c r="D24" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D25" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D26" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E26" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D27" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D28" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
-        <v>33</v>
+      <c r="D29" s="2">
+        <v>6.54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="2">
+        <v>46.38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2">
+        <v>41.2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="2">
+        <v>199.9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="2">
+        <v>780</v>
+      </c>
+      <c r="E36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="2">
+        <v>68.22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -749,9 +1334,7 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -770,9 +1353,7 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>